<commit_message>
Update Character Select Screen
</commit_message>
<xml_diff>
--- a/OtherFiles/ControlScheme.xlsx
+++ b/OtherFiles/ControlScheme.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolo4\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\[1]_Work\Macromedia\Sonstiges\Initiativprojekt\catchAndChaosGitHub\OtherFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09ADCA5-478B-486D-A1A9-38DA0DB8D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6EA22F-47B5-46A2-9DFC-B0A83A5B5519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="25720" windowHeight="20970" xr2:uid="{5BBD0571-C6C3-4597-A857-3568ED1290BB}"/>
+    <workbookView xWindow="6740" yWindow="2090" windowWidth="28800" windowHeight="15370" xr2:uid="{5BBD0571-C6C3-4597-A857-3568ED1290BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
   <si>
     <t>Controls</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Take / Throw Plushie</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Parent</t>
   </si>
 </sst>
 </file>
@@ -474,15 +486,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B6BDD7-FA52-4CF7-94C9-4ABB4E502982}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31" x14ac:dyDescent="0.7">
@@ -560,74 +572,96 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>11</v>
+      <c r="A10" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>